<commit_message>
Drawing costs to separate file (plotCosts.py) Paramater for evaluating/not model every so many iterations while training and putting results to a file
</commit_message>
<xml_diff>
--- a/results.20180510.5.xlsx
+++ b/results.20180510.5.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">results!$A$1:$K$51</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -1123,8 +1123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>